<commit_message>
calibrate mcglt to allow for more cap builds
</commit_message>
<xml_diff>
--- a/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
+++ b/InputData/elec/MCGLT/Max Cap Growth Lookup Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Wisconsin\WI_model\InputData\elec\MCGLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7331728-2E0D-48BA-8B8E-23ADE57FBBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BB0092-969F-49F4-BAA1-8FE347C90D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="840" windowWidth="17580" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="2130" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1576,7 +1576,7 @@
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,11 +1611,11 @@
         <v>109</v>
       </c>
       <c r="C2" s="5">
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D2" s="5">
         <f>C2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
@@ -1639,11 +1639,11 @@
       </c>
       <c r="C4" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D4" s="5">
         <f>C4</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
@@ -1667,11 +1667,11 @@
       </c>
       <c r="C6" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D6" s="4">
         <f>C6</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
@@ -1695,11 +1695,11 @@
       </c>
       <c r="C8" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D8" s="4">
         <f>C8</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
@@ -1727,11 +1727,11 @@
       </c>
       <c r="C10" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D10" s="5">
         <f>C10</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1794,11 +1794,11 @@
       </c>
       <c r="C12" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D12" s="5">
         <f>C12</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
@@ -1855,11 +1855,11 @@
       </c>
       <c r="C14" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D14" s="4">
         <f>C14</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
@@ -1883,11 +1883,11 @@
       </c>
       <c r="C16" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D16" s="4">
         <f>C16</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,12 +1910,11 @@
         <v>109</v>
       </c>
       <c r="C18" s="5">
-        <f>$C$2</f>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
         <f>C18</f>
-        <v>800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,11 +1938,11 @@
       </c>
       <c r="C20" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D20" s="4">
         <f>C20</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,11 +1966,11 @@
       </c>
       <c r="C22" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D22" s="4">
         <f>C22</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1995,11 +1994,11 @@
       </c>
       <c r="C24" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D24" s="1">
         <f>C24</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,7 +2049,7 @@
       </c>
       <c r="C28" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
@@ -2077,7 +2076,7 @@
       </c>
       <c r="C30" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -2104,11 +2103,11 @@
       </c>
       <c r="C32" s="5">
         <f>$C$2</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
       <c r="D32" s="4">
         <f>C32</f>
-        <v>800</v>
+        <v>3500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>